<commit_message>
refactored code, set formatting style, cleaned comments, set dependencies & packages to be in correct locations and included
</commit_message>
<xml_diff>
--- a/invTester.xlsx
+++ b/invTester.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\git\Inventory\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="invTest" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>CommaStart</t>
   </si>
@@ -36,9 +31,6 @@
     <t>//Title1</t>
   </si>
   <si>
-    <t>ItemA</t>
-  </si>
-  <si>
     <t>UnitA</t>
   </si>
   <si>
@@ -46,6 +38,21 @@
   </si>
   <si>
     <t>UnitB</t>
+  </si>
+  <si>
+    <t>ItemC</t>
+  </si>
+  <si>
+    <t>UnitC</t>
+  </si>
+  <si>
+    <t>UnitD</t>
+  </si>
+  <si>
+    <t>ItemD</t>
+  </si>
+  <si>
+    <t>Item,A</t>
   </si>
 </sst>
 </file>
@@ -632,7 +639,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -667,7 +674,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -844,7 +851,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -852,11 +859,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
@@ -879,10 +888,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -896,10 +905,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -909,6 +918,40 @@
       </c>
       <c r="E4">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>